<commit_message>
changes in whole sale and add min max script
</commit_message>
<xml_diff>
--- a/CartRules_1123.xlsx
+++ b/CartRules_1123.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,13 +399,35 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2422</v>
+        <v>13928</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>5151</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>13928</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes in the main scripts
</commit_message>
<xml_diff>
--- a/CartRules_1123.xlsx
+++ b/CartRules_1123.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,35 +399,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>13928</v>
+        <v>7630</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>5151</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>13928</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>